<commit_message>
Added annotated waveform diagrams. Updated document
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300E9C3B-4573-42A4-812D-F3AF8B4AAA6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA32F4C-B333-4B04-9B5C-59B398140B6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>Helped teammates debug VHDL implementation for ArithUnit.vhd and Adder.vhd.</t>
+  </si>
+  <si>
+    <t>Begin annotation of waveform diagrams for LogicUnit.vhd</t>
+  </si>
+  <si>
+    <t>Updated document. Added annotated waveform diagrams to document.</t>
   </si>
 </sst>
 </file>
@@ -721,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G757"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45:G45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,18 +1473,38 @@
       </c>
     </row>
     <row r="46" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="11"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="18"/>
-      <c r="G46" s="11"/>
+      <c r="B46" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C46" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D46" s="16">
+        <v>9.375E-2</v>
+      </c>
+      <c r="E46" s="18">
+        <v>0.13541666666666666</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="47" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="11"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="18"/>
-      <c r="G47" s="11"/>
+      <c r="B47" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C47" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D47" s="16">
+        <v>0.13541666666666666</v>
+      </c>
+      <c r="E47" s="18">
+        <v>0.15625</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="48" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="11"/>

</xml_diff>

<commit_message>
Fixed VHDL code in Adder.vhd, ArithUnit.vhd and LogicUnit.vhd
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-6977-350-1201.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA32F4C-B333-4B04-9B5C-59B398140B6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AD46F8-8B4E-48E4-AB66-0E1A7C7EFC6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -189,6 +191,21 @@
   </si>
   <si>
     <t>Updated document. Added annotated waveform diagrams to document.</t>
+  </si>
+  <si>
+    <t>Provided tech support to give team members access to Github repository</t>
+  </si>
+  <si>
+    <t>Reviewed team mates' work on Arith.vhd, Adder.vhd and related files</t>
+  </si>
+  <si>
+    <t>Fixed formatting of Arith.vhd and Adder.vhd.</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Removed unnecessary VHDL code from LogicUnit.vhd.</t>
   </si>
 </sst>
 </file>
@@ -725,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
-  <dimension ref="A1:G757"/>
+  <dimension ref="A1:G764"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,58 +1524,141 @@
       </c>
     </row>
     <row r="48" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="11"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="18"/>
-      <c r="G48" s="11"/>
-    </row>
-    <row r="49" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="11"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="18"/>
-      <c r="G49" s="11"/>
-    </row>
-    <row r="50" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="11"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="18"/>
-      <c r="G50" s="11"/>
-    </row>
-    <row r="51" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="11"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="16"/>
+      <c r="B48" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C48" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D48" s="16">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E48" s="18">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C49" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D49" s="16">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="E49" s="18">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C50" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D50" s="16">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="E50" s="18">
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C51" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D51" s="16">
+        <v>0.64236111111111105</v>
+      </c>
       <c r="E51" s="18"/>
-      <c r="G51" s="11"/>
-    </row>
-    <row r="52" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G51" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="11"/>
       <c r="C52" s="9"/>
       <c r="D52" s="16"/>
       <c r="E52" s="18"/>
       <c r="G52" s="11"/>
     </row>
-    <row r="53" spans="2:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="12"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="19"/>
-      <c r="G53" s="12"/>
-    </row>
-    <row r="54" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="11"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="18"/>
+      <c r="G53" s="11"/>
+    </row>
+    <row r="54" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="11"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="18"/>
+      <c r="G54" s="11"/>
+    </row>
+    <row r="55" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="11"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="18"/>
+      <c r="G55" s="11"/>
+    </row>
+    <row r="56" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="11"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="18"/>
+      <c r="G56" s="11"/>
+    </row>
+    <row r="57" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="11"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="18"/>
+      <c r="G57" s="11"/>
+    </row>
+    <row r="58" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="11"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="18"/>
+      <c r="G58" s="11"/>
+    </row>
+    <row r="59" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="11"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="18"/>
+      <c r="G59" s="11"/>
+    </row>
+    <row r="60" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="12"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="19"/>
+      <c r="G60" s="12"/>
+    </row>
+    <row r="61" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2252,6 +2352,13 @@
     <row r="755" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="756" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="757" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:D1"/>

</xml_diff>

<commit_message>
Recompiled all .vhd files. Updated summary, .vho and .sdo files
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AD46F8-8B4E-48E4-AB66-0E1A7C7EFC6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F47A3D-1F8E-4E65-91F3-8CA8BFB26A55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -206,6 +206,15 @@
   </si>
   <si>
     <t>Removed unnecessary VHDL code from LogicUnit.vhd.</t>
+  </si>
+  <si>
+    <t>Validated and verified waveforms for ArithUnit.vhd and Adder.vhd</t>
+  </si>
+  <si>
+    <t>Re-compiled VHDL code for LogicUnit.vhd, Adder.vhd and ArithUnit.vhd</t>
+  </si>
+  <si>
+    <t>Updated all summary files, .vho files and .sdo files.</t>
   </si>
 </sst>
 </file>
@@ -744,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G764"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,31 +1596,63 @@
       <c r="D51" s="16">
         <v>0.64236111111111105</v>
       </c>
-      <c r="E51" s="18"/>
+      <c r="E51" s="18">
+        <v>0.64930555555555558</v>
+      </c>
       <c r="G51" s="11" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="11"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="18"/>
-      <c r="G52" s="11"/>
+      <c r="B52" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C52" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D52" s="16">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="E52" s="18">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="11"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="18"/>
-      <c r="G53" s="11"/>
+      <c r="B53" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C53" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D53" s="16">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="E53" s="18">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="11"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="18"/>
-      <c r="G54" s="11"/>
+      <c r="B54" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C54" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D54" s="16">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="E54" s="18">
+        <v>0.77916666666666667</v>
+      </c>
+      <c r="G54" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="11"/>

</xml_diff>

<commit_message>
Tidied up own log file
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F47A3D-1F8E-4E65-91F3-8CA8BFB26A55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2EBDC1-CCF4-40E3-828E-76B022F3DD46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -136,51 +136,18 @@
     <t>Fixed ArithUnit.vhd and Adder.vhd so they compile on ModelSim and Quartus.</t>
   </si>
   <si>
-    <t>Fixed ArithUnit.vhd and Adder.vhd such that both .do scripts work (previosuly they do not work as pointed out by my teammates). Each script works if and only if all ports are defined properly</t>
-  </si>
-  <si>
     <t>Generated the functional waveforms of the LogicUnit.vhd. Exported them into Documentation as per instructions</t>
   </si>
   <si>
-    <t>Systhesied circuits but not satisfied with the diagrams due to it being very cluttered. Will grab the images later when a revised version is done</t>
-  </si>
-  <si>
-    <t>Set up files and environment to obtain timing simulations from ModelSim</t>
-  </si>
-  <si>
-    <t>Updated .gitignore to ignore temporary files that is unneeded</t>
-  </si>
-  <si>
-    <t>Obtained timing waveforms and added them to Documentation as per instructions.</t>
-  </si>
-  <si>
-    <t>Added TestVectors. Discovered a bug in LogicUnit.vhd. Stopped for dinner</t>
-  </si>
-  <si>
     <t>Fixed LogicUnit.vhd.</t>
   </si>
   <si>
-    <t>Created RTL netlist images and Post-fit images</t>
-  </si>
-  <si>
-    <t>Updated Timing waveforms for LogicUnit.vhd</t>
-  </si>
-  <si>
-    <t>Updated Functional Waveforms for LogicUnit.vhd</t>
-  </si>
-  <si>
     <t>Updated folder structure of Documentation directory. Started working on the report.</t>
   </si>
   <si>
     <t>Added overview sections of LogicUnit to report. Noticed that Truth table documented is different than VHDL code</t>
   </si>
   <si>
-    <t>Re-compiled VHDL code</t>
-  </si>
-  <si>
-    <t>Renamed .vho and .sdo files for LogicUnit. Exported .vho, .sdo, .map.summary and .fit.summary files to Documentation folder of LogicUnit</t>
-  </si>
-  <si>
     <t>Added waveforms for LogicUnit.vhd to document</t>
   </si>
   <si>
@@ -190,31 +157,73 @@
     <t>Begin annotation of waveform diagrams for LogicUnit.vhd</t>
   </si>
   <si>
-    <t>Updated document. Added annotated waveform diagrams to document.</t>
-  </si>
-  <si>
     <t>Provided tech support to give team members access to Github repository</t>
   </si>
   <si>
-    <t>Reviewed team mates' work on Arith.vhd, Adder.vhd and related files</t>
-  </si>
-  <si>
-    <t>Fixed formatting of Arith.vhd and Adder.vhd.</t>
-  </si>
-  <si>
     <t>s</t>
   </si>
   <si>
-    <t>Removed unnecessary VHDL code from LogicUnit.vhd.</t>
-  </si>
-  <si>
-    <t>Validated and verified waveforms for ArithUnit.vhd and Adder.vhd</t>
-  </si>
-  <si>
-    <t>Re-compiled VHDL code for LogicUnit.vhd, Adder.vhd and ArithUnit.vhd</t>
-  </si>
-  <si>
-    <t>Updated all summary files, .vho files and .sdo files.</t>
+    <t>Removed .gitignore rule for transcript files.</t>
+  </si>
+  <si>
+    <t>Validated and verified waveforms for ArithUnit.vhd and Adder.vhd. DONE</t>
+  </si>
+  <si>
+    <t>Re-compiled VHDL code for LogicUnit.vhd, Adder.vhd and ArithUnit.vhd. DONE</t>
+  </si>
+  <si>
+    <t>Updated all summary files, .vho files and .sdo files. DONE</t>
+  </si>
+  <si>
+    <t>Updated .gitignore to ignore transcript files</t>
+  </si>
+  <si>
+    <t>Obtained timing waveforms and added them to Documentation as per instructions. DONE</t>
+  </si>
+  <si>
+    <t>Updated Functional Waveforms for LogicUnit.vhd. DONE</t>
+  </si>
+  <si>
+    <t>Created RTL netlist images and Post-fit images. DONE</t>
+  </si>
+  <si>
+    <t>Updated Timing waveforms for LogicUnit.vhd. DONE</t>
+  </si>
+  <si>
+    <t>Renamed .vho and .sdo files for LogicUnit. Exported .vho, .sdo, .map.summary and .fit.summary files to Documentation folder of LogicUnit. DONE</t>
+  </si>
+  <si>
+    <t>Updated document. Added annotated waveform diagrams to document. Will continue work on document tomorrow</t>
+  </si>
+  <si>
+    <t>Reviewing team mates' work on Arith.vhd, Adder.vhd and related files. Discovered things that need to be changed.</t>
+  </si>
+  <si>
+    <t>Fixed formatting of Arith.vhd and Adder.vhd. Removed unnecessary comments. DONE</t>
+  </si>
+  <si>
+    <t>Removed unnecessary VHDL code from LogicUnit.vhd. DONE</t>
+  </si>
+  <si>
+    <t>Fixed ArithUnit.vhd and Adder.vhd such that both .do scripts work (previosuly they do not work as pointed out by my teammates). Each script works if and only if all ports are defined properly. DONE</t>
+  </si>
+  <si>
+    <t>Set up files and environment to obtain timing simulations from ModelSim. DONE</t>
+  </si>
+  <si>
+    <t>Added TestVectors. Discovered a bug in LogicUnit.vhd before stopping for dinner.</t>
+  </si>
+  <si>
+    <t>Systhesied circuits. Will grab the images later.</t>
+  </si>
+  <si>
+    <t>Re-compiled VHDL code for LogicUnit.vhd. DONE</t>
+  </si>
+  <si>
+    <t>Re-formatted and edited own log file to make it tidier.</t>
+  </si>
+  <si>
+    <t>Consolidated all files except for report document into one folder to get ready for submission.</t>
   </si>
 </sst>
 </file>
@@ -753,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G764"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1198,7 @@
         <v>0.96875</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1206,7 +1215,7 @@
         <v>0.98958333333333337</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1223,7 +1232,7 @@
         <v>0.99652777777777779</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1240,7 +1249,7 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1257,7 +1266,7 @@
         <v>4.8611111111111112E-3</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1274,7 +1283,7 @@
         <v>1.5972222222222224E-2</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1291,7 +1300,7 @@
         <v>0.75763888888888886</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1308,7 +1317,7 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1325,7 +1334,7 @@
         <v>0.94791666666666663</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1342,7 +1351,7 @@
         <v>0.96180555555555547</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1359,7 +1368,7 @@
         <v>0.97916666666666663</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1376,7 +1385,7 @@
         <v>0.98749999999999993</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1393,7 +1402,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1410,7 +1419,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1427,7 +1436,7 @@
         <v>3.6111111111111115E-2</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1444,7 +1453,7 @@
         <v>5.9722222222222225E-2</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1461,7 +1470,7 @@
         <v>6.8749999999999992E-2</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1478,7 +1487,7 @@
         <v>7.4305555555555555E-2</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1495,7 +1504,7 @@
         <v>9.375E-2</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1512,7 +1521,7 @@
         <v>0.13541666666666666</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1529,7 +1538,7 @@
         <v>0.15625</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1546,7 +1555,7 @@
         <v>0.61805555555555558</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1585,7 +1594,7 @@
     </row>
     <row r="51" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B51" s="11">
         <v>6977</v>
@@ -1600,7 +1609,7 @@
         <v>0.64930555555555558</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1617,7 +1626,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1634,7 +1643,7 @@
         <v>0.76041666666666663</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1651,36 +1660,76 @@
         <v>0.77916666666666667</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="11"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="18"/>
-      <c r="G55" s="11"/>
+      <c r="B55" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C55" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D55" s="16">
+        <v>0.77916666666666667</v>
+      </c>
+      <c r="E55" s="18">
+        <v>0.78611111111111109</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="56" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="11"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="18"/>
-      <c r="G56" s="11"/>
+      <c r="B56" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C56" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D56" s="16">
+        <v>0.78611111111111109</v>
+      </c>
+      <c r="E56" s="18">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="57" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="11"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="18"/>
-      <c r="G57" s="11"/>
+      <c r="B57" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C57" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D57" s="16">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E57" s="18">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="58" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="11"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="18"/>
-      <c r="G58" s="11"/>
+      <c r="B58" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C58" s="9">
+        <v>43926</v>
+      </c>
+      <c r="D58" s="16">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="E58" s="18">
+        <v>0.80833333333333324</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="59" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="11"/>

</xml_diff>

<commit_message>
Re-checked all files. Re-compiled VHD files. Updated all documents and updated submission folder
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C375D7A8-9670-4371-A5BB-520A8DD2E3D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB401D1A-95D8-4BAA-B718-E514F076C3DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>Verified project download works on a fresh installation of the project. Teammates had discovered this issue earlier and is a source of a massive headache.</t>
+  </si>
+  <si>
+    <t>Re-compiled all VHD files and checked that all results are the same. Updated transcript , summary, .vho and .sdo files. DONE</t>
   </si>
 </sst>
 </file>
@@ -777,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G772"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1825,9 +1828,15 @@
       <c r="C63" s="9">
         <v>43926</v>
       </c>
-      <c r="D63" s="16"/>
-      <c r="E63" s="18"/>
-      <c r="G63" s="11"/>
+      <c r="D63" s="16">
+        <v>0.86041666666666661</v>
+      </c>
+      <c r="E63" s="18">
+        <v>0.88194444444444453</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="64" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="11">

</xml_diff>

<commit_message>
Updated log files. Added student number
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G47-6977-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G47-6977-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBC8F8D-672C-4233-9186-0570553C07B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFD58D2-8296-43AE-8D52-04F7ED4E8E55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15330" yWindow="3585" windowWidth="21600" windowHeight="11385" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G772"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1852,7 +1852,7 @@
         <v>0.90347222222222223</v>
       </c>
       <c r="E64" s="18">
-        <v>0.91180555555555554</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="G64" s="11" t="s">
         <v>66</v>

</xml_diff>